<commit_message>
Made a graph for kpl
</commit_message>
<xml_diff>
--- a/LacTissueLooserBounds.xlsx
+++ b/LacTissueLooserBounds.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\MATLAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D97509D4-D29C-43D3-BCD9-96C6FCBD61EF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B832E58B-3052-4DA3-BF97-122A1D3FDFA7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2F20C6FD-021A-4423-86E6-4420FC1D340E}"/>
   </bookViews>
@@ -113,6 +113,884 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$I$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>kPL</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$J$21:$M$21</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>HK-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>UMRC6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>UOK262</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>UOK+DIDS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$J$22:$M$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>4.4543679214273189E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.8065354275440272E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.9910694114928816E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.2350313360057905E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-368A-4259-BBB8-4A39937F969B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="476071264"/>
+        <c:axId val="563629392"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="476071264"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="563629392"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="563629392"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="476071264"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>601980</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>34290</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>297180</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>34290</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{81705905-4F46-4776-B58C-01B70426C126}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -415,7 +1293,7 @@
   <dimension ref="A1:Q39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="M39" sqref="M39"/>
+      <selection activeCell="M32" sqref="M32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -980,7 +1858,7 @@
         <v>1</v>
       </c>
       <c r="B17">
-        <f t="shared" ref="B17:F26" si="0">IF(OR(ABS(B1-M$5)&lt;=0.001*M$5,ABS(B1-M$6)&lt;=0.001*M$6),0,1)</f>
+        <f t="shared" ref="B17:F17" si="0">IF(OR(ABS(B1-M$5)&lt;=0.001*M$5,ABS(B1-M$6)&lt;=0.001*M$6),0,1)</f>
         <v>1</v>
       </c>
       <c r="C17">
@@ -1722,5 +2600,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Made some graphs of what happened to cell data when using tissue slice model and lowering R1 to 0.1 AKA T1Lin to 10
</commit_message>
<xml_diff>
--- a/LacTissueLooserBounds.xlsx
+++ b/LacTissueLooserBounds.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\MATLAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B832E58B-3052-4DA3-BF97-122A1D3FDFA7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD6B218E-282D-435C-AA2F-337CC9A7797D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2F20C6FD-021A-4423-86E6-4420FC1D340E}"/>
   </bookViews>
@@ -185,11 +185,157 @@
               <a:schemeClr val="accent1"/>
             </a:solidFill>
             <a:ln>
-              <a:noFill/>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000000-2384-49FF-971A-E4B98196AE06}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-2384-49FF-971A-E4B98196AE06}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-2384-49FF-971A-E4B98196AE06}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-2384-49FF-971A-E4B98196AE06}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet1!$J$23:$M$23</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>3.2957560791630532E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1.3191149923296716E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>2.5375092468312428E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>4.4930929757617463E-3</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet1!$J$23:$M$23</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>3.2957560791630532E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1.3191149923296716E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>2.5375092468312428E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>4.4930929757617463E-3</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$J$21:$M$21</c:f>
@@ -409,6 +555,446 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$M$38</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>kLEfflux</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-EACE-4D1C-B749-9B0C77502BD9}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-EACE-4D1C-B749-9B0C77502BD9}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-EACE-4D1C-B749-9B0C77502BD9}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000004-EACE-4D1C-B749-9B0C77502BD9}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet1!$N$39:$Q$39</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>9.5172341727416173E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.2762556298764825</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.20742890262357622</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.23320788970097311</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet1!$N$39:$Q$39</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>9.5172341727416173E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.2762556298764825</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.20742890262357622</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.23320788970097311</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$N$37:$Q$37</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>HK-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>UMRC6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>UOK262</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>UOK+DIDS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$N$38:$Q$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>7.4700453467023267E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.46545965253624355</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.4310535245442722</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.3028650275580253</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-EACE-4D1C-B749-9B0C77502BD9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="623423560"/>
+        <c:axId val="623424544"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="623423560"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="623424544"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="623424544"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="623423560"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -449,7 +1035,550 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -985,6 +2114,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>26670</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>26670</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A5CC767D-1AF4-4C98-A5CF-CDBEE2434BC5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1292,8 +2457,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D6ED431-84FC-4407-BD4F-865BEB101693}">
   <dimension ref="A1:Q39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="M32" sqref="M32"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>